<commit_message>
added logic to calculate word score
</commit_message>
<xml_diff>
--- a/공 굴리기_info_word.xlsx
+++ b/공 굴리기_info_word.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choeseung-u/unity/FortuneRunner/ASO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EDBF1F-7EC1-3840-9175-CF25B19D2153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41529D0-3654-C546-974C-804428BC8E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1818,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L448"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>

</xml_diff>